<commit_message>
bug: pdf creation in progress
</commit_message>
<xml_diff>
--- a/src/main/resources/Labels/newLabel/retourLabel.xlsx
+++ b/src/main/resources/Labels/newLabel/retourLabel.xlsx
@@ -224,22 +224,22 @@
     <t>HollandHaag BV</t>
   </si>
   <si>
-    <t>vincent</t>
-  </si>
-  <si>
-    <t>Orin 15</t>
-  </si>
-  <si>
-    <t>MD-3652</t>
-  </si>
-  <si>
-    <t>AKEMI CS-4377-150</t>
+    <t>mustafa</t>
+  </si>
+  <si>
+    <t>Northview 1</t>
+  </si>
+  <si>
+    <t>4342</t>
+  </si>
+  <si>
+    <t>AKEMI CS-3355-150</t>
   </si>
   <si>
     <t>akemi</t>
   </si>
   <si>
-    <t>4377</t>
+    <t>3355</t>
   </si>
   <si>
     <t>length: 5.0  width: 0.0</t>

</xml_diff>

<commit_message>
ALTERED: Reüploaded labels from resources, removed unused classes from constructor in ArticleControllerV2 and removed bean cycle in ArticleOrderController.
</commit_message>
<xml_diff>
--- a/src/main/resources/Labels/newLabel/retourLabel.xlsx
+++ b/src/main/resources/Labels/newLabel/retourLabel.xlsx
@@ -224,22 +224,22 @@
     <t>HollandHaag BV</t>
   </si>
   <si>
-    <t>mustafa</t>
-  </si>
-  <si>
-    <t>Northview 1</t>
-  </si>
-  <si>
-    <t>4342</t>
-  </si>
-  <si>
-    <t>AKEMI CS-3355-150</t>
+    <t>sjoerd</t>
+  </si>
+  <si>
+    <t>Hallows 26</t>
+  </si>
+  <si>
+    <t>7006</t>
+  </si>
+  <si>
+    <t>AKEMI CS-3746-150</t>
   </si>
   <si>
     <t>akemi</t>
   </si>
   <si>
-    <t>3355</t>
+    <t>3746</t>
   </si>
   <si>
     <t>length: 5.0  width: 0.0</t>

</xml_diff>